<commit_message>
Adicionado o controle de status para Atividade
- Validacao: Antes de editar uma atividade, o admin deve Desativar ela
- Layout: atividades inativas ficam brancas
- CRUD: adicionado o attr status ao criar e editar uma atividade
</commit_message>
<xml_diff>
--- a/public/DadosParaKalango - SemFormulas.xlsx
+++ b/public/DadosParaKalango - SemFormulas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9210" windowHeight="7080" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9210" windowHeight="7080" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Idiomas" sheetId="5" r:id="rId1"/>
@@ -8420,7 +8420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -8475,14 +8475,14 @@
       </c>
       <c r="G2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(RANDBETWEEN(1,30),$A$1:$B$31,2,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Odete Ishida</v>
+        <v>Rafaela Matos</v>
       </c>
       <c r="H2" t="s">
         <v>201</v>
       </c>
       <c r="I2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(RANDBETWEEN(1,20),$A$1:$C$21,3,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Caio Castanheira</v>
+        <v>Eric Pádua</v>
       </c>
       <c r="J2" t="s">
         <v>196</v>
@@ -8503,14 +8503,14 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G66" ca="1" si="0">CONCATENATE(VLOOKUP(RANDBETWEEN(1,30),$A$1:$B$31,2,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Andreia Sato</v>
+        <v>Angelina Hernandes</v>
       </c>
       <c r="H3" t="s">
         <v>201</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I66" ca="1" si="1">CONCATENATE(VLOOKUP(RANDBETWEEN(1,20),$A$1:$C$21,3,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Claudio Costa</v>
+        <v>Augusto Yamada</v>
       </c>
       <c r="J3" t="s">
         <v>196</v>
@@ -8531,14 +8531,14 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Caroline Nazário</v>
+        <v>Irene Faria</v>
       </c>
       <c r="H4" t="s">
         <v>201</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Doulgas Suzuki</v>
+        <v>Claudio Alves</v>
       </c>
       <c r="J4" t="s">
         <v>196</v>
@@ -8559,14 +8559,14 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bruna Takahashi</v>
+        <v>Monica Faria</v>
       </c>
       <c r="H5" t="s">
         <v>201</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Otavio da Silva</v>
+        <v>Yori Gouveia</v>
       </c>
       <c r="J5" t="s">
         <v>196</v>
@@ -8587,14 +8587,14 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Michele Takahashi</v>
+        <v>Lara Suzuki</v>
       </c>
       <c r="H6" t="s">
         <v>201</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Filipe Takahashi</v>
+        <v>Doulgas Neto</v>
       </c>
       <c r="J6" t="s">
         <v>196</v>
@@ -8615,14 +8615,14 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Milena Suzuki</v>
+        <v>Kitana Freire</v>
       </c>
       <c r="H7" t="s">
         <v>201</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Fernando da Silva</v>
+        <v>Cleber Valverde</v>
       </c>
       <c r="J7" t="s">
         <v>196</v>
@@ -8643,14 +8643,14 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Akemi Monteiro</v>
+        <v>Monica Neto</v>
       </c>
       <c r="H8" t="s">
         <v>201</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eduardo Pádua</v>
+        <v>Filipe Semedo</v>
       </c>
       <c r="J8" t="s">
         <v>196</v>
@@ -8671,14 +8671,14 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Irene Neto</v>
+        <v>Akemi Rocha</v>
       </c>
       <c r="H9" t="s">
         <v>201</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cauê Jordão</v>
+        <v>Xerxes Redfield</v>
       </c>
       <c r="J9" t="s">
         <v>196</v>
@@ -8699,14 +8699,14 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Kitana Neves</v>
+        <v>Sarah Alves</v>
       </c>
       <c r="H10" t="s">
         <v>201</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Filipe Takahashi</v>
+        <v>Otavio Faria</v>
       </c>
       <c r="J10" t="s">
         <v>196</v>
@@ -8727,14 +8727,14 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Barbara Peixoto</v>
+        <v>Yoko Rocha</v>
       </c>
       <c r="H11" t="s">
         <v>201</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cauê Villablanca</v>
+        <v>Dante Carvalho</v>
       </c>
       <c r="J11" t="s">
         <v>196</v>
@@ -8755,14 +8755,14 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yoko Carvalho</v>
+        <v>Monica Villablanca</v>
       </c>
       <c r="H12" t="s">
         <v>201</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Jaime Neves</v>
+        <v>Caio Lins</v>
       </c>
       <c r="J12" t="s">
         <v>196</v>
@@ -8783,14 +8783,14 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ChunLi Macedo</v>
+        <v>Andreia Valverde</v>
       </c>
       <c r="H13" t="s">
         <v>201</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cauê Severo</v>
+        <v>Claudio Macedo</v>
       </c>
       <c r="J13" t="s">
         <v>196</v>
@@ -8811,14 +8811,14 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Michele Camilo</v>
+        <v>Jill Semedo</v>
       </c>
       <c r="H14" t="s">
         <v>201</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cauê dos Santos</v>
+        <v>Eric Franca</v>
       </c>
       <c r="J14" t="s">
         <v>196</v>
@@ -8839,14 +8839,14 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Monica Gouveia</v>
+        <v>ChunLi Yamada</v>
       </c>
       <c r="H15" t="s">
         <v>201</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eduardo Redfield</v>
+        <v>Eric Severo</v>
       </c>
       <c r="J15" t="s">
         <v>196</v>
@@ -8867,14 +8867,14 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Irene Valverde</v>
+        <v>Aline Semedo</v>
       </c>
       <c r="H16" t="s">
         <v>201</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eduardo Batista</v>
+        <v>Leonidas Salgueiro</v>
       </c>
       <c r="J16" t="s">
         <v>196</v>
@@ -8895,14 +8895,14 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alexandra Tanaka</v>
+        <v>Tamires Camilo</v>
       </c>
       <c r="H17" t="s">
         <v>201</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Jaime Nazário</v>
+        <v>Eric Severo</v>
       </c>
       <c r="J17" t="s">
         <v>196</v>
@@ -8923,14 +8923,14 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Monica Jordão</v>
+        <v>Irene da Silva</v>
       </c>
       <c r="H18" t="s">
         <v>201</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Fernando Peixoto</v>
+        <v>Peterson Pinheiro</v>
       </c>
       <c r="J18" t="s">
         <v>196</v>
@@ -8951,14 +8951,14 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bruna Macedo</v>
+        <v>Irene Pinheiro</v>
       </c>
       <c r="H19" t="s">
         <v>201</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cleber Faria</v>
+        <v>Augusto Pádua</v>
       </c>
       <c r="J19" t="s">
         <v>196</v>
@@ -8979,14 +8979,14 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bruna dos Santos</v>
+        <v>Aline Yamada</v>
       </c>
       <c r="H20" t="s">
         <v>201</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cleber Takahashi</v>
+        <v>Dante Neves</v>
       </c>
       <c r="J20" t="s">
         <v>196</v>
@@ -9007,14 +9007,14 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Kitana Freire</v>
+        <v>Tamires Takahashi</v>
       </c>
       <c r="H21" t="s">
         <v>201</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Yori Salgueiro</v>
+        <v>Leonidas Costa</v>
       </c>
       <c r="J21" t="s">
         <v>196</v>
@@ -9032,14 +9032,14 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Odete Pinheiro</v>
+        <v>Caroline Costa</v>
       </c>
       <c r="H22" t="s">
         <v>201</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cleber Costa</v>
+        <v>Eric Lins</v>
       </c>
       <c r="J22" t="s">
         <v>196</v>
@@ -9057,14 +9057,14 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Odete Faria</v>
+        <v>Odete Semedo</v>
       </c>
       <c r="H23" t="s">
         <v>201</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Augusto Matos</v>
+        <v>Jaime Redfield</v>
       </c>
       <c r="J23" t="s">
         <v>196</v>
@@ -9082,14 +9082,14 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Kitana Pádua</v>
+        <v>Lara Faria</v>
       </c>
       <c r="H24" t="s">
         <v>201</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Filipe Carvalho</v>
+        <v>Filipe Tanaka</v>
       </c>
       <c r="J24" t="s">
         <v>196</v>
@@ -9107,14 +9107,14 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Camila Neves</v>
+        <v>Milena Neto</v>
       </c>
       <c r="H25" t="s">
         <v>201</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eric Freire</v>
+        <v>Yori Hernandes</v>
       </c>
       <c r="J25" t="s">
         <v>196</v>
@@ -9132,14 +9132,14 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angelina Leal</v>
+        <v>Kitana Matos</v>
       </c>
       <c r="H26" t="s">
         <v>201</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Xerxes Salgueiro</v>
+        <v>Augusto Alves</v>
       </c>
       <c r="J26" t="s">
         <v>196</v>
@@ -9157,14 +9157,14 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Jill Rocha</v>
+        <v>Odete Macedo</v>
       </c>
       <c r="H27" t="s">
         <v>201</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Fernando Freire</v>
+        <v>Fernando Takahashi</v>
       </c>
       <c r="J27" t="s">
         <v>196</v>
@@ -9182,14 +9182,14 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Angelina Freire</v>
+        <v>Angelina Sato</v>
       </c>
       <c r="H28" t="s">
         <v>201</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Caio Franca</v>
+        <v>Simão Villablanca</v>
       </c>
       <c r="J28" t="s">
         <v>196</v>
@@ -9207,14 +9207,14 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rafaela Leal</v>
+        <v>Angelina Jordão</v>
       </c>
       <c r="H29" t="s">
         <v>201</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Yori Monteiro</v>
+        <v>Augusto Rocha</v>
       </c>
       <c r="J29" t="s">
         <v>196</v>
@@ -9232,14 +9232,14 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Jonas Torres</v>
+        <v>Barbara Freire</v>
       </c>
       <c r="H30" t="s">
         <v>201</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Yori Castanheira</v>
+        <v>Morpheu Tanaka</v>
       </c>
       <c r="J30" t="s">
         <v>196</v>
@@ -9257,14 +9257,14 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yoko Semedo</v>
+        <v>Irene Alves</v>
       </c>
       <c r="H31" t="s">
         <v>201</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eduardo da Silva</v>
+        <v>Otavio Lins</v>
       </c>
       <c r="J31" t="s">
         <v>196</v>
@@ -9279,14 +9279,14 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Michele Pinheiro</v>
+        <v>Yoko Takahashi</v>
       </c>
       <c r="H32" t="s">
         <v>201</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Filipe Sato</v>
+        <v>Leonidas Sato</v>
       </c>
       <c r="J32" t="s">
         <v>196</v>
@@ -9301,14 +9301,14 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Camila Freire</v>
+        <v>Odete Sato</v>
       </c>
       <c r="H33" t="s">
         <v>201</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Augusto Yamada</v>
+        <v>Doulgas Peixoto</v>
       </c>
       <c r="J33" t="s">
         <v>196</v>
@@ -9323,14 +9323,14 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Michele Monteiro</v>
+        <v>Rafaela Takahashi</v>
       </c>
       <c r="H34" t="s">
         <v>201</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cauê Tanaka</v>
+        <v>Cleber Severo</v>
       </c>
       <c r="J34" t="s">
         <v>196</v>
@@ -9345,14 +9345,14 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rafaela Tanaka</v>
+        <v>Tamires Nazário</v>
       </c>
       <c r="H35" t="s">
         <v>201</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cleber Valverde</v>
+        <v>Jaime Semedo</v>
       </c>
       <c r="J35" t="s">
         <v>196</v>
@@ -9367,14 +9367,14 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alexandra Pinheiro</v>
+        <v>Sonia Peixoto</v>
       </c>
       <c r="H36" t="s">
         <v>201</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eric Alves</v>
+        <v>Eric Jordão</v>
       </c>
       <c r="J36" t="s">
         <v>196</v>
@@ -9389,14 +9389,14 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Jade Peixoto</v>
+        <v>Monica Suzuki</v>
       </c>
       <c r="H37" t="s">
         <v>201</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Simão Alves</v>
+        <v>Xerxes Gouveia</v>
       </c>
       <c r="J37" t="s">
         <v>196</v>
@@ -9411,14 +9411,14 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Fernanda Salgueiro</v>
+        <v>Jéssica Neto</v>
       </c>
       <c r="H38" t="s">
         <v>201</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Xerxes Castanheira</v>
+        <v>Bruno Faria</v>
       </c>
       <c r="J38" t="s">
         <v>196</v>
@@ -9433,14 +9433,14 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alexandra Salgueiro</v>
+        <v>Tamires Matos</v>
       </c>
       <c r="H39" t="s">
         <v>201</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Claudio Faria</v>
+        <v>Fernando Valentine</v>
       </c>
       <c r="J39" t="s">
         <v>196</v>
@@ -9455,14 +9455,14 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Alexandra Lins</v>
+        <v>Tamires Takahashi</v>
       </c>
       <c r="H40" t="s">
         <v>201</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Peterson Neto</v>
+        <v>Fernando Franca</v>
       </c>
       <c r="J40" t="s">
         <v>196</v>
@@ -9477,14 +9477,14 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Akemi Faria</v>
+        <v>Caroline Camilo</v>
       </c>
       <c r="H41" t="s">
         <v>201</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eduardo Costa</v>
+        <v>Claudio Semedo</v>
       </c>
       <c r="J41" t="s">
         <v>196</v>
@@ -9499,14 +9499,14 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Akemi Macedo</v>
+        <v>Monica Alves</v>
       </c>
       <c r="H42" t="s">
         <v>201</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Dante Suzuki</v>
+        <v>Leonidas Monteiro</v>
       </c>
       <c r="J42" t="s">
         <v>196</v>
@@ -9521,14 +9521,14 @@
       </c>
       <c r="G43" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Irene Valverde</v>
+        <v>ChunLi Semedo</v>
       </c>
       <c r="H43" t="s">
         <v>201</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Dante Minazuki</v>
+        <v>Yori Camilo</v>
       </c>
       <c r="J43" t="s">
         <v>196</v>
@@ -9543,14 +9543,14 @@
       </c>
       <c r="G44" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Akemi dos Santos</v>
+        <v>Bruna Minazuki</v>
       </c>
       <c r="H44" t="s">
         <v>201</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Peterson Salgueiro</v>
+        <v>Doulgas Alves</v>
       </c>
       <c r="J44" t="s">
         <v>196</v>
@@ -9565,14 +9565,14 @@
       </c>
       <c r="G45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Odete Neves</v>
+        <v>Monica Costa</v>
       </c>
       <c r="H45" t="s">
         <v>201</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cleber Sato</v>
+        <v>Morpheu Yamada</v>
       </c>
       <c r="J45" t="s">
         <v>196</v>
@@ -9587,14 +9587,14 @@
       </c>
       <c r="G46" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Milena Nazário</v>
+        <v>Jonas Franca</v>
       </c>
       <c r="H46" t="s">
         <v>201</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Otavio dos Santos</v>
+        <v>Leonidas Batista</v>
       </c>
       <c r="J46" t="s">
         <v>196</v>
@@ -9603,14 +9603,14 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G47" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Caroline Lins</v>
+        <v>Monica Torres</v>
       </c>
       <c r="H47" t="s">
         <v>201</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Caio Jordão</v>
+        <v>Cleber Neto</v>
       </c>
       <c r="J47" t="s">
         <v>196</v>
@@ -9619,14 +9619,14 @@
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G48" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Camila Jordão</v>
+        <v>Akemi Faria</v>
       </c>
       <c r="H48" t="s">
         <v>201</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eric Macedo</v>
+        <v>Filipe Sato</v>
       </c>
       <c r="J48" t="s">
         <v>196</v>
@@ -9635,14 +9635,14 @@
     <row r="49" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G49" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Aline Peixoto</v>
+        <v>Fernanda Gouveia</v>
       </c>
       <c r="H49" t="s">
         <v>201</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Caio Alves</v>
+        <v>Dante Villablanca</v>
       </c>
       <c r="J49" t="s">
         <v>196</v>
@@ -9651,14 +9651,14 @@
     <row r="50" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G50" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Fernanda Takahashi</v>
+        <v>Odete Suzuki</v>
       </c>
       <c r="H50" t="s">
         <v>201</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Caio Neves</v>
+        <v>Augusto Lins</v>
       </c>
       <c r="J50" t="s">
         <v>196</v>
@@ -9667,14 +9667,14 @@
     <row r="51" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G51" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lara Rocha</v>
+        <v>Irene Gouveia</v>
       </c>
       <c r="H51" t="s">
         <v>201</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Yori Takahashi</v>
+        <v>Otavio Carvalho</v>
       </c>
       <c r="J51" t="s">
         <v>196</v>
@@ -9683,14 +9683,14 @@
     <row r="52" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G52" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Aline Nazário</v>
+        <v>Yoko dos Santos</v>
       </c>
       <c r="H52" t="s">
         <v>201</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Claudio Semedo</v>
+        <v>Caio Macedo</v>
       </c>
       <c r="J52" t="s">
         <v>196</v>
@@ -9699,14 +9699,14 @@
     <row r="53" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G53" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Monica Takahashi</v>
+        <v>Yoko Faria</v>
       </c>
       <c r="H53" t="s">
         <v>201</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Simão Gouveia</v>
+        <v>Caio Neto</v>
       </c>
       <c r="J53" t="s">
         <v>196</v>
@@ -9715,14 +9715,14 @@
     <row r="54" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Trinity Alves</v>
+        <v>Alexandra Hernandes</v>
       </c>
       <c r="H54" t="s">
         <v>201</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Cauê Sato</v>
+        <v>Doulgas Valentine</v>
       </c>
       <c r="J54" t="s">
         <v>196</v>
@@ -9731,14 +9731,14 @@
     <row r="55" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G55" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sarah Villablanca</v>
+        <v>Lara da Silva</v>
       </c>
       <c r="H55" t="s">
         <v>201</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Fernando Alves</v>
+        <v>Morpheu Torres</v>
       </c>
       <c r="J55" t="s">
         <v>196</v>
@@ -9747,14 +9747,14 @@
     <row r="56" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G56" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Akemi Carvalho</v>
+        <v>Lara dos Santos</v>
       </c>
       <c r="H56" t="s">
         <v>201</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Morpheu Salgueiro</v>
+        <v>Eric Alves</v>
       </c>
       <c r="J56" t="s">
         <v>196</v>
@@ -9763,14 +9763,14 @@
     <row r="57" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G57" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Trinity Castanheira</v>
+        <v>Sheeva Franca</v>
       </c>
       <c r="H57" t="s">
         <v>201</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Doulgas Ishida</v>
+        <v>Cleber Suzuki</v>
       </c>
       <c r="J57" t="s">
         <v>196</v>
@@ -9779,14 +9779,14 @@
     <row r="58" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G58" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Aline Neto</v>
+        <v>Daniela Suzuki</v>
       </c>
       <c r="H58" t="s">
         <v>201</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Morpheu Takahashi</v>
+        <v>Leonidas Salgueiro</v>
       </c>
       <c r="J58" t="s">
         <v>196</v>
@@ -9795,14 +9795,14 @@
     <row r="59" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G59" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Daniela Suzuki</v>
+        <v>Rafaela Pinheiro</v>
       </c>
       <c r="H59" t="s">
         <v>201</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Caio Suzuki</v>
+        <v>Fernando Leal</v>
       </c>
       <c r="J59" t="s">
         <v>196</v>
@@ -9811,14 +9811,14 @@
     <row r="60" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G60" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Barbara Freire</v>
+        <v>Rafaela Valentine</v>
       </c>
       <c r="H60" t="s">
         <v>201</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Fernando Macedo</v>
+        <v>Yori Lins</v>
       </c>
       <c r="J60" t="s">
         <v>196</v>
@@ -9827,14 +9827,14 @@
     <row r="61" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G61" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Kitana Leal</v>
+        <v>Akemi Castanheira</v>
       </c>
       <c r="H61" t="s">
         <v>201</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Eric Semedo</v>
+        <v>Yori Valverde</v>
       </c>
       <c r="J61" t="s">
         <v>196</v>
@@ -9843,14 +9843,14 @@
     <row r="62" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G62" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Kitana Carvalho</v>
+        <v>Lara da Silva</v>
       </c>
       <c r="H62" t="s">
         <v>201</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Morpheu Ishida</v>
+        <v>Leonidas Salgueiro</v>
       </c>
       <c r="J62" t="s">
         <v>196</v>
@@ -9859,14 +9859,14 @@
     <row r="63" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G63" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Trinity Castanheira</v>
+        <v>Sheeva Neves</v>
       </c>
       <c r="H63" t="s">
         <v>201</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Doulgas Pinheiro</v>
+        <v>Cleber Carvalho</v>
       </c>
       <c r="J63" t="s">
         <v>196</v>
@@ -9875,14 +9875,14 @@
     <row r="64" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G64" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lara Gouveia</v>
+        <v>Kitana Faria</v>
       </c>
       <c r="H64" t="s">
         <v>201</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Dante Yamada</v>
+        <v>Jaime Matos</v>
       </c>
       <c r="J64" t="s">
         <v>196</v>
@@ -9891,14 +9891,14 @@
     <row r="65" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G65" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tamires Yamada</v>
+        <v>Jéssica Takahashi</v>
       </c>
       <c r="H65" t="s">
         <v>201</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Yori Hernandes</v>
+        <v>Cauê Matos</v>
       </c>
       <c r="J65" t="s">
         <v>196</v>
@@ -9907,14 +9907,14 @@
     <row r="66" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G66" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rafaela Faria</v>
+        <v>Andreia Alves</v>
       </c>
       <c r="H66" t="s">
         <v>201</v>
       </c>
       <c r="I66" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Dante Suzuki</v>
+        <v>Bruno Yamada</v>
       </c>
       <c r="J66" t="s">
         <v>196</v>
@@ -9923,14 +9923,14 @@
     <row r="67" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G67" t="str">
         <f t="shared" ref="G67:G131" ca="1" si="2">CONCATENATE(VLOOKUP(RANDBETWEEN(1,30),$A$1:$B$31,2,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Caroline Severo</v>
+        <v>Jéssica Alves</v>
       </c>
       <c r="H67" t="s">
         <v>201</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I131" ca="1" si="3">CONCATENATE(VLOOKUP(RANDBETWEEN(1,20),$A$1:$C$21,3,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Claudio Suzuki</v>
+        <v>Jaime Faria</v>
       </c>
       <c r="J67" t="s">
         <v>196</v>
@@ -9939,14 +9939,14 @@
     <row r="68" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G68" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Michele Villablanca</v>
+        <v>Lara Lins</v>
       </c>
       <c r="H68" t="s">
         <v>201</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Claudio Semedo</v>
+        <v>Xerxes Matos</v>
       </c>
       <c r="J68" t="s">
         <v>196</v>
@@ -9955,14 +9955,14 @@
     <row r="69" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G69" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Barbara Batista</v>
+        <v>Jonas Faria</v>
       </c>
       <c r="H69" t="s">
         <v>201</v>
       </c>
       <c r="I69" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Cleber Salgueiro</v>
+        <v>Dante Yamada</v>
       </c>
       <c r="J69" t="s">
         <v>196</v>
@@ -9971,14 +9971,14 @@
     <row r="70" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G70" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ChunLi Neves</v>
+        <v>Jéssica Castanheira</v>
       </c>
       <c r="H70" t="s">
         <v>201</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Claudio Monteiro</v>
+        <v>Yori dos Santos</v>
       </c>
       <c r="J70" t="s">
         <v>196</v>
@@ -9987,14 +9987,14 @@
     <row r="71" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G71" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Angelina Alves</v>
+        <v>Fernanda Gouveia</v>
       </c>
       <c r="H71" t="s">
         <v>201</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Peterson dos Santos</v>
+        <v>Caio Rocha</v>
       </c>
       <c r="J71" t="s">
         <v>196</v>
@@ -10003,14 +10003,14 @@
     <row r="72" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G72" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Alexandra Ishida</v>
+        <v>Milena Semedo</v>
       </c>
       <c r="H72" t="s">
         <v>201</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Jaime Villablanca</v>
+        <v>Cleber Jordão</v>
       </c>
       <c r="J72" t="s">
         <v>196</v>
@@ -10019,14 +10019,14 @@
     <row r="73" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G73" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Akemi Camilo</v>
+        <v>Bruna Redfield</v>
       </c>
       <c r="H73" t="s">
         <v>201</v>
       </c>
       <c r="I73" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Dante Redfield</v>
+        <v>Eduardo Yamada</v>
       </c>
       <c r="J73" t="s">
         <v>196</v>
@@ -10035,14 +10035,14 @@
     <row r="74" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G74" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Monica Nazário</v>
+        <v>Akemi Severo</v>
       </c>
       <c r="H74" t="s">
         <v>201</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Caio dos Santos</v>
+        <v>Simão Leal</v>
       </c>
       <c r="J74" t="s">
         <v>196</v>
@@ -10051,14 +10051,14 @@
     <row r="75" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G75" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Sheeva Valentine</v>
+        <v>Alexandra Ishida</v>
       </c>
       <c r="H75" t="s">
         <v>201</v>
       </c>
       <c r="I75" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Augusto Sato</v>
+        <v>Doulgas dos Santos</v>
       </c>
       <c r="J75" t="s">
         <v>196</v>
@@ -10067,14 +10067,14 @@
     <row r="76" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G76" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Fernanda da Silva</v>
+        <v>Aline Carvalho</v>
       </c>
       <c r="H76" t="s">
         <v>201</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Simão Takahashi</v>
+        <v>Fernando Faria</v>
       </c>
       <c r="J76" t="s">
         <v>196</v>
@@ -10083,14 +10083,14 @@
     <row r="77" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G77" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Odete Suzuki</v>
+        <v>Caroline Costa</v>
       </c>
       <c r="H77" t="s">
         <v>201</v>
       </c>
       <c r="I77" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Eduardo Faria</v>
+        <v>Morpheu Sato</v>
       </c>
       <c r="J77" t="s">
         <v>196</v>
@@ -10099,14 +10099,14 @@
     <row r="78" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G78" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Milena Rocha</v>
+        <v>Alexandra Gouveia</v>
       </c>
       <c r="H78" t="s">
         <v>201</v>
       </c>
       <c r="I78" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Cauê Severo</v>
+        <v>Filipe Nazário</v>
       </c>
       <c r="J78" t="s">
         <v>196</v>
@@ -10115,14 +10115,14 @@
     <row r="79" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G79" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Tamires Franca</v>
+        <v>Sarah Freire</v>
       </c>
       <c r="H79" t="s">
         <v>201</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Augusto Faria</v>
+        <v>Augusto Lins</v>
       </c>
       <c r="J79" t="s">
         <v>196</v>
@@ -10131,14 +10131,14 @@
     <row r="80" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G80" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Akemi Freire</v>
+        <v>Caroline Semedo</v>
       </c>
       <c r="H80" t="s">
         <v>201</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Cauê Alves</v>
+        <v>Eduardo Gouveia</v>
       </c>
       <c r="J80" t="s">
         <v>196</v>
@@ -10147,14 +10147,14 @@
     <row r="81" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G81" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Caroline Minazuki</v>
+        <v>Sarah Castanheira</v>
       </c>
       <c r="H81" t="s">
         <v>201</v>
       </c>
       <c r="I81" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Xerxes Takahashi</v>
+        <v>Simão Torres</v>
       </c>
       <c r="J81" t="s">
         <v>196</v>
@@ -10163,14 +10163,14 @@
     <row r="82" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G82" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ChunLi Faria</v>
+        <v>Jéssica Neto</v>
       </c>
       <c r="H82" t="s">
         <v>201</v>
       </c>
       <c r="I82" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Doulgas Monteiro</v>
+        <v>Cauê Valverde</v>
       </c>
       <c r="J82" t="s">
         <v>196</v>
@@ -10179,14 +10179,14 @@
     <row r="83" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G83" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Milena Costa</v>
+        <v>Tamires Castanheira</v>
       </c>
       <c r="H83" t="s">
         <v>201</v>
       </c>
       <c r="I83" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Dante Alves</v>
+        <v>Eric Jordão</v>
       </c>
       <c r="J83" t="s">
         <v>196</v>
@@ -10195,14 +10195,14 @@
     <row r="84" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G84" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Angelina Sato</v>
+        <v>Daniela Pádua</v>
       </c>
       <c r="H84" t="s">
         <v>201</v>
       </c>
       <c r="I84" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Filipe Valentine</v>
+        <v>Doulgas Freire</v>
       </c>
       <c r="J84" t="s">
         <v>196</v>
@@ -10211,14 +10211,14 @@
     <row r="85" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G85" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Camila dos Santos</v>
+        <v>Trinity Ishida</v>
       </c>
       <c r="H85" t="s">
         <v>201</v>
       </c>
       <c r="I85" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Simão Ishida</v>
+        <v>Caio Minazuki</v>
       </c>
       <c r="J85" t="s">
         <v>196</v>
@@ -10227,14 +10227,14 @@
     <row r="86" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G86" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Kitana Neto</v>
+        <v>Tamires Rocha</v>
       </c>
       <c r="H86" t="s">
         <v>201</v>
       </c>
       <c r="I86" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Filipe Nazário</v>
+        <v>Cauê Peixoto</v>
       </c>
       <c r="J86" t="s">
         <v>196</v>
@@ -10243,14 +10243,14 @@
     <row r="87" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G87" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Irene Camilo</v>
+        <v>Aline Redfield</v>
       </c>
       <c r="H87" t="s">
         <v>201</v>
       </c>
       <c r="I87" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Fernando Matos</v>
+        <v>Cleber Peixoto</v>
       </c>
       <c r="J87" t="s">
         <v>196</v>
@@ -10259,14 +10259,14 @@
     <row r="88" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G88" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Aline Villablanca</v>
+        <v>Sarah Macedo</v>
       </c>
       <c r="H88" t="s">
         <v>201</v>
       </c>
       <c r="I88" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Yori Camilo</v>
+        <v>Simão Valverde</v>
       </c>
       <c r="J88" t="s">
         <v>196</v>
@@ -10275,14 +10275,14 @@
     <row r="89" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G89" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Alexandra da Silva</v>
+        <v>Irene Minazuki</v>
       </c>
       <c r="H89" t="s">
         <v>201</v>
       </c>
       <c r="I89" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Filipe Carvalho</v>
+        <v>Fernando Pinheiro</v>
       </c>
       <c r="J89" t="s">
         <v>196</v>
@@ -10291,14 +10291,14 @@
     <row r="90" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G90" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Jill Valverde</v>
+        <v>Daniela Monteiro</v>
       </c>
       <c r="H90" t="s">
         <v>201</v>
       </c>
       <c r="I90" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Fernando Jordão</v>
+        <v>Cauê Camilo</v>
       </c>
       <c r="J90" t="s">
         <v>196</v>
@@ -10307,14 +10307,14 @@
     <row r="91" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G91" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ChunLi Faria</v>
+        <v>Akemi Rocha</v>
       </c>
       <c r="H91" t="s">
         <v>201</v>
       </c>
       <c r="I91" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Claudio Batista</v>
+        <v>Yori Takahashi</v>
       </c>
       <c r="J91" t="s">
         <v>196</v>
@@ -10323,14 +10323,14 @@
     <row r="92" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G92" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Barbara Ishida</v>
+        <v>Angelina Takahashi</v>
       </c>
       <c r="H92" t="s">
         <v>201</v>
       </c>
       <c r="I92" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Peterson Valverde</v>
+        <v>Cleber Faria</v>
       </c>
       <c r="J92" t="s">
         <v>196</v>
@@ -10339,14 +10339,14 @@
     <row r="93" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G93" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Sarah Semedo</v>
+        <v>Kitana Pádua</v>
       </c>
       <c r="H93" t="s">
         <v>201</v>
       </c>
       <c r="I93" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Simão Carvalho</v>
+        <v>Filipe Matos</v>
       </c>
       <c r="J93" t="s">
         <v>196</v>
@@ -10355,14 +10355,14 @@
     <row r="94" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G94" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Jill Jordão</v>
+        <v>Jéssica Sato</v>
       </c>
       <c r="H94" t="s">
         <v>201</v>
       </c>
       <c r="I94" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Caio Redfield</v>
+        <v>Peterson Neto</v>
       </c>
       <c r="J94" t="s">
         <v>196</v>
@@ -10371,14 +10371,14 @@
     <row r="95" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G95" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Jéssica Pinheiro</v>
+        <v>Aline Valentine</v>
       </c>
       <c r="H95" t="s">
         <v>201</v>
       </c>
       <c r="I95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Fernando Faria</v>
+        <v>Bruno Neves</v>
       </c>
       <c r="J95" t="s">
         <v>196</v>
@@ -10387,14 +10387,14 @@
     <row r="96" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G96" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Lara Peixoto</v>
+        <v>Daniela Franca</v>
       </c>
       <c r="H96" t="s">
         <v>201</v>
       </c>
       <c r="I96" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Caio Takahashi</v>
+        <v>Xerxes Yamada</v>
       </c>
       <c r="J96" t="s">
         <v>196</v>
@@ -10403,14 +10403,14 @@
     <row r="97" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G97" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Milena Valentine</v>
+        <v>Lara Neto</v>
       </c>
       <c r="H97" t="s">
         <v>201</v>
       </c>
       <c r="I97" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Fernando Neto</v>
+        <v>Caio Macedo</v>
       </c>
       <c r="J97" t="s">
         <v>196</v>
@@ -10419,14 +10419,14 @@
     <row r="98" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G98" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Camila Salgueiro</v>
+        <v>Milena Tanaka</v>
       </c>
       <c r="H98" t="s">
         <v>201</v>
       </c>
       <c r="I98" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Claudio Valverde</v>
+        <v>Caio Leal</v>
       </c>
       <c r="J98" t="s">
         <v>196</v>
@@ -10435,14 +10435,14 @@
     <row r="99" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G99" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Kitana Faria</v>
+        <v>Lara Carvalho</v>
       </c>
       <c r="H99" t="s">
         <v>201</v>
       </c>
       <c r="I99" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Dante Costa</v>
+        <v>Doulgas Torres</v>
       </c>
       <c r="J99" t="s">
         <v>196</v>
@@ -10451,14 +10451,14 @@
     <row r="100" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G100" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Andreia Gouveia</v>
+        <v>Odete Franca</v>
       </c>
       <c r="H100" t="s">
         <v>201</v>
       </c>
       <c r="I100" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Augusto Ishida</v>
+        <v>Filipe Macedo</v>
       </c>
       <c r="J100" t="s">
         <v>196</v>
@@ -10467,14 +10467,14 @@
     <row r="101" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G101" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Michele Pinheiro</v>
+        <v>Akemi Takahashi</v>
       </c>
       <c r="H101" t="s">
         <v>201</v>
       </c>
       <c r="I101" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Cleber Torres</v>
+        <v>Doulgas Rocha</v>
       </c>
       <c r="J101" t="s">
         <v>196</v>
@@ -10483,14 +10483,14 @@
     <row r="102" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G102" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Rafaela Hernandes</v>
+        <v>Milena Redfield</v>
       </c>
       <c r="H102" t="s">
         <v>201</v>
       </c>
       <c r="I102" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Jaime Macedo</v>
+        <v>Xerxes Freire</v>
       </c>
       <c r="J102" t="s">
         <v>196</v>
@@ -10499,14 +10499,14 @@
     <row r="103" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G103" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Monica Salgueiro</v>
+        <v>Jill Suzuki</v>
       </c>
       <c r="H103" t="s">
         <v>201</v>
       </c>
       <c r="I103" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Caio Suzuki</v>
+        <v>Otavio Monteiro</v>
       </c>
       <c r="J103" t="s">
         <v>196</v>
@@ -10515,14 +10515,14 @@
     <row r="104" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G104" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Michele Leal</v>
+        <v>Caroline Jordão</v>
       </c>
       <c r="H104" t="s">
         <v>201</v>
       </c>
       <c r="I104" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Augusto Peixoto</v>
+        <v>Peterson Alves</v>
       </c>
       <c r="J104" t="s">
         <v>196</v>
@@ -10531,14 +10531,14 @@
     <row r="105" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G105" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Angelina Minazuki</v>
+        <v>Camila Redfield</v>
       </c>
       <c r="H105" t="s">
         <v>201</v>
       </c>
       <c r="I105" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Yori Hernandes</v>
+        <v>Xerxes Faria</v>
       </c>
       <c r="J105" t="s">
         <v>196</v>
@@ -10547,14 +10547,14 @@
     <row r="106" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G106" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Milena Alves</v>
+        <v>Lara Suzuki</v>
       </c>
       <c r="H106" t="s">
         <v>201</v>
       </c>
       <c r="I106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Dante Faria</v>
+        <v>Simão Neves</v>
       </c>
       <c r="J106" t="s">
         <v>196</v>
@@ -10563,14 +10563,14 @@
     <row r="107" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G107" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Kitana Severo</v>
+        <v>Lara Nazário</v>
       </c>
       <c r="H107" t="s">
         <v>201</v>
       </c>
       <c r="I107" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Eric Camilo</v>
+        <v>Yori Sato</v>
       </c>
       <c r="J107" t="s">
         <v>196</v>
@@ -10579,14 +10579,14 @@
     <row r="108" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G108" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Daniela Takahashi</v>
+        <v>Milena Neto</v>
       </c>
       <c r="H108" t="s">
         <v>201</v>
       </c>
       <c r="I108" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Leonidas Batista</v>
+        <v>Jaime Lins</v>
       </c>
       <c r="J108" t="s">
         <v>196</v>
@@ -10595,14 +10595,14 @@
     <row r="109" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G109" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Trinity Neto</v>
+        <v>Trinity Tanaka</v>
       </c>
       <c r="H109" t="s">
         <v>201</v>
       </c>
       <c r="I109" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Augusto Carvalho</v>
+        <v>Simão da Silva</v>
       </c>
       <c r="J109" t="s">
         <v>196</v>
@@ -10611,14 +10611,14 @@
     <row r="110" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G110" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Sheeva da Silva</v>
+        <v>Rafaela Carvalho</v>
       </c>
       <c r="H110" t="s">
         <v>201</v>
       </c>
       <c r="I110" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Caio Camilo</v>
+        <v>Doulgas Franca</v>
       </c>
       <c r="J110" t="s">
         <v>196</v>
@@ -10627,14 +10627,14 @@
     <row r="111" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G111" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Monica Lins</v>
+        <v>Yoko Takahashi</v>
       </c>
       <c r="H111" t="s">
         <v>201</v>
       </c>
       <c r="I111" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Simão Peixoto</v>
+        <v>Bruno Takahashi</v>
       </c>
       <c r="J111" t="s">
         <v>196</v>
@@ -10643,14 +10643,14 @@
     <row r="112" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G112" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Sheeva Batista</v>
+        <v>Caroline dos Santos</v>
       </c>
       <c r="H112" t="s">
         <v>201</v>
       </c>
       <c r="I112" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Caio Minazuki</v>
+        <v>Simão Torres</v>
       </c>
       <c r="J112" t="s">
         <v>196</v>
@@ -10659,14 +10659,14 @@
     <row r="113" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G113" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Daniela Suzuki</v>
+        <v>Jill Castanheira</v>
       </c>
       <c r="H113" t="s">
         <v>201</v>
       </c>
       <c r="I113" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Leonidas Neto</v>
+        <v>Dante Camilo</v>
       </c>
       <c r="J113" t="s">
         <v>196</v>
@@ -10675,14 +10675,14 @@
     <row r="114" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G114" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Jonas Valverde</v>
+        <v>Sarah Sato</v>
       </c>
       <c r="H114" t="s">
         <v>201</v>
       </c>
       <c r="I114" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Eduardo Neto</v>
+        <v>Simão Costa</v>
       </c>
       <c r="J114" t="s">
         <v>196</v>
@@ -10691,14 +10691,14 @@
     <row r="115" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G115" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Alexandra Peixoto</v>
+        <v>Yoko Severo</v>
       </c>
       <c r="H115" t="s">
         <v>201</v>
       </c>
       <c r="I115" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Augusto Jordão</v>
+        <v>Dante Valentine</v>
       </c>
       <c r="J115" t="s">
         <v>196</v>
@@ -10707,14 +10707,14 @@
     <row r="116" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G116" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Kitana Torres</v>
+        <v>Michele Salgueiro</v>
       </c>
       <c r="H116" t="s">
         <v>201</v>
       </c>
       <c r="I116" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Leonidas Hernandes</v>
+        <v>Eric Valentine</v>
       </c>
       <c r="J116" t="s">
         <v>196</v>
@@ -10723,14 +10723,14 @@
     <row r="117" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G117" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Aline Redfield</v>
+        <v>Jill Faria</v>
       </c>
       <c r="H117" t="s">
         <v>201</v>
       </c>
       <c r="I117" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Otavio Suzuki</v>
+        <v>Caio Villablanca</v>
       </c>
       <c r="J117" t="s">
         <v>196</v>
@@ -10739,14 +10739,14 @@
     <row r="118" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G118" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Fernanda Faria</v>
+        <v>Akemi Costa</v>
       </c>
       <c r="H118" t="s">
         <v>201</v>
       </c>
       <c r="I118" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Xerxes Ishida</v>
+        <v>Jaime Takahashi</v>
       </c>
       <c r="J118" t="s">
         <v>196</v>
@@ -10755,14 +10755,14 @@
     <row r="119" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G119" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Jéssica Valentine</v>
+        <v>Jill dos Santos</v>
       </c>
       <c r="H119" t="s">
         <v>201</v>
       </c>
       <c r="I119" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Simão Nazário</v>
+        <v>Augusto Ishida</v>
       </c>
       <c r="J119" t="s">
         <v>196</v>
@@ -10771,14 +10771,14 @@
     <row r="120" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G120" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Sonia Sato</v>
+        <v>Alexandra Alves</v>
       </c>
       <c r="H120" t="s">
         <v>201</v>
       </c>
       <c r="I120" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Caio Alves</v>
+        <v>Filipe Camilo</v>
       </c>
       <c r="J120" t="s">
         <v>196</v>
@@ -10787,14 +10787,14 @@
     <row r="121" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G121" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Trinity Monteiro</v>
+        <v>ChunLi dos Santos</v>
       </c>
       <c r="H121" t="s">
         <v>201</v>
       </c>
       <c r="I121" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Bruno Neto</v>
+        <v>Morpheu Leal</v>
       </c>
       <c r="J121" t="s">
         <v>196</v>
@@ -10803,14 +10803,14 @@
     <row r="122" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G122" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Sonia Freire</v>
+        <v>Sarah Leal</v>
       </c>
       <c r="H122" t="s">
         <v>201</v>
       </c>
       <c r="I122" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Doulgas dos Santos</v>
+        <v>Caio Faria</v>
       </c>
       <c r="J122" t="s">
         <v>196</v>
@@ -10819,14 +10819,14 @@
     <row r="123" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G123" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Daniela Peixoto</v>
+        <v>Aline Jordão</v>
       </c>
       <c r="H123" t="s">
         <v>201</v>
       </c>
       <c r="I123" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Otavio Peixoto</v>
+        <v>Xerxes Jordão</v>
       </c>
       <c r="J123" t="s">
         <v>196</v>
@@ -10835,14 +10835,14 @@
     <row r="124" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G124" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Tamires Hernandes</v>
+        <v>Milena Neves</v>
       </c>
       <c r="H124" t="s">
         <v>201</v>
       </c>
       <c r="I124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Yori Monteiro</v>
+        <v>Claudio Castanheira</v>
       </c>
       <c r="J124" t="s">
         <v>196</v>
@@ -10851,14 +10851,14 @@
     <row r="125" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G125" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Daniela dos Santos</v>
+        <v>Bruna Costa</v>
       </c>
       <c r="H125" t="s">
         <v>201</v>
       </c>
       <c r="I125" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Yori da Silva</v>
+        <v>Dante Ishida</v>
       </c>
       <c r="J125" t="s">
         <v>196</v>
@@ -10867,14 +10867,14 @@
     <row r="126" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G126" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Michele Alves</v>
+        <v>Sheeva Rocha</v>
       </c>
       <c r="H126" t="s">
         <v>201</v>
       </c>
       <c r="I126" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Dante Alves</v>
+        <v>Yori Costa</v>
       </c>
       <c r="J126" t="s">
         <v>196</v>
@@ -10883,14 +10883,14 @@
     <row r="127" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G127" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Caroline Jordão</v>
+        <v>Daniela Sato</v>
       </c>
       <c r="H127" t="s">
         <v>201</v>
       </c>
       <c r="I127" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Simão Franca</v>
+        <v>Doulgas Rocha</v>
       </c>
       <c r="J127" t="s">
         <v>196</v>
@@ -10899,14 +10899,14 @@
     <row r="128" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G128" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Fernanda Pádua</v>
+        <v>Aline Camilo</v>
       </c>
       <c r="H128" t="s">
         <v>201</v>
       </c>
       <c r="I128" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Claudio Faria</v>
+        <v>Caio Neto</v>
       </c>
       <c r="J128" t="s">
         <v>196</v>
@@ -10915,14 +10915,14 @@
     <row r="129" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G129" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Sheeva Neves</v>
+        <v>Kitana Freire</v>
       </c>
       <c r="H129" t="s">
         <v>201</v>
       </c>
       <c r="I129" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Cleber Matos</v>
+        <v>Filipe Takahashi</v>
       </c>
       <c r="J129" t="s">
         <v>196</v>
@@ -10931,14 +10931,14 @@
     <row r="130" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G130" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Jill Severo</v>
+        <v>Trinity Neto</v>
       </c>
       <c r="H130" t="s">
         <v>201</v>
       </c>
       <c r="I130" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Morpheu Villablanca</v>
+        <v>Morpheu Camilo</v>
       </c>
       <c r="J130" t="s">
         <v>196</v>
@@ -10947,14 +10947,14 @@
     <row r="131" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G131" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Akemi Faria</v>
+        <v>Odete Sato</v>
       </c>
       <c r="H131" t="s">
         <v>201</v>
       </c>
       <c r="I131" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Simão Sato</v>
+        <v>Eric Alves</v>
       </c>
       <c r="J131" t="s">
         <v>196</v>
@@ -10963,14 +10963,14 @@
     <row r="132" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G132" t="str">
         <f t="shared" ref="G132:G195" ca="1" si="4">CONCATENATE(VLOOKUP(RANDBETWEEN(1,30),$A$1:$B$31,2,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Daniela Peixoto</v>
+        <v>Kitana Minazuki</v>
       </c>
       <c r="H132" t="s">
         <v>201</v>
       </c>
       <c r="I132" t="str">
         <f t="shared" ref="I132:I195" ca="1" si="5">CONCATENATE(VLOOKUP(RANDBETWEEN(1,20),$A$1:$C$21,3,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Eric Minazuki</v>
+        <v>Augusto Sato</v>
       </c>
       <c r="J132" t="s">
         <v>196</v>
@@ -10979,14 +10979,14 @@
     <row r="133" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G133" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Jonas Nazário</v>
+        <v>Milena Rocha</v>
       </c>
       <c r="H133" t="s">
         <v>201</v>
       </c>
       <c r="I133" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Doulgas Camilo</v>
+        <v>Eric Leal</v>
       </c>
       <c r="J133" t="s">
         <v>196</v>
@@ -10995,14 +10995,14 @@
     <row r="134" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G134" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Jonas Severo</v>
+        <v>Michele Jordão</v>
       </c>
       <c r="H134" t="s">
         <v>201</v>
       </c>
       <c r="I134" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Peterson Alves</v>
+        <v>Yori da Silva</v>
       </c>
       <c r="J134" t="s">
         <v>196</v>
@@ -11011,14 +11011,14 @@
     <row r="135" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G135" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Akemi Castanheira</v>
+        <v>Odete Castanheira</v>
       </c>
       <c r="H135" t="s">
         <v>201</v>
       </c>
       <c r="I135" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Morpheu Peixoto</v>
+        <v>Otavio Redfield</v>
       </c>
       <c r="J135" t="s">
         <v>196</v>
@@ -11027,14 +11027,14 @@
     <row r="136" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G136" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Rafaela Matos</v>
+        <v>Odete Batista</v>
       </c>
       <c r="H136" t="s">
         <v>201</v>
       </c>
       <c r="I136" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Morpheu Franca</v>
+        <v>Augusto Sato</v>
       </c>
       <c r="J136" t="s">
         <v>196</v>
@@ -11043,14 +11043,14 @@
     <row r="137" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G137" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Tamires Valentine</v>
+        <v>Michele Takahashi</v>
       </c>
       <c r="H137" t="s">
         <v>201</v>
       </c>
       <c r="I137" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Otavio Batista</v>
+        <v>Cleber Macedo</v>
       </c>
       <c r="J137" t="s">
         <v>196</v>
@@ -11059,14 +11059,14 @@
     <row r="138" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G138" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Jill Leal</v>
+        <v>Sonia Alves</v>
       </c>
       <c r="H138" t="s">
         <v>201</v>
       </c>
       <c r="I138" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Claudio Sato</v>
+        <v>Morpheu Macedo</v>
       </c>
       <c r="J138" t="s">
         <v>196</v>
@@ -11075,14 +11075,14 @@
     <row r="139" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G139" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Kitana Ishida</v>
+        <v>Alexandra Neto</v>
       </c>
       <c r="H139" t="s">
         <v>201</v>
       </c>
       <c r="I139" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Leonidas Redfield</v>
+        <v>Augusto Nazário</v>
       </c>
       <c r="J139" t="s">
         <v>196</v>
@@ -11091,14 +11091,14 @@
     <row r="140" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G140" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Aline Torres</v>
+        <v>Sonia Carvalho</v>
       </c>
       <c r="H140" t="s">
         <v>201</v>
       </c>
       <c r="I140" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Cleber Ishida</v>
+        <v>Augusto Franca</v>
       </c>
       <c r="J140" t="s">
         <v>196</v>
@@ -11107,14 +11107,14 @@
     <row r="141" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G141" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Akemi Leal</v>
+        <v>Rafaela Villablanca</v>
       </c>
       <c r="H141" t="s">
         <v>201</v>
       </c>
       <c r="I141" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Bruno Jordão</v>
+        <v>Morpheu Franca</v>
       </c>
       <c r="J141" t="s">
         <v>196</v>
@@ -11123,14 +11123,14 @@
     <row r="142" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G142" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Tamires Neto</v>
+        <v>Lara Macedo</v>
       </c>
       <c r="H142" t="s">
         <v>201</v>
       </c>
       <c r="I142" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Otavio Neto</v>
+        <v>Claudio Pádua</v>
       </c>
       <c r="J142" t="s">
         <v>196</v>
@@ -11139,14 +11139,14 @@
     <row r="143" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G143" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Fernanda Takahashi</v>
+        <v>Tamires Franca</v>
       </c>
       <c r="H143" t="s">
         <v>201</v>
       </c>
       <c r="I143" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Cleber Gouveia</v>
+        <v>Fernando Faria</v>
       </c>
       <c r="J143" t="s">
         <v>196</v>
@@ -11155,14 +11155,14 @@
     <row r="144" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G144" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Yoko Matos</v>
+        <v>Jonas Faria</v>
       </c>
       <c r="H144" t="s">
         <v>201</v>
       </c>
       <c r="I144" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Dante Ishida</v>
+        <v>Peterson Redfield</v>
       </c>
       <c r="J144" t="s">
         <v>196</v>
@@ -11171,14 +11171,14 @@
     <row r="145" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G145" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Lara Hernandes</v>
+        <v>Michele Suzuki</v>
       </c>
       <c r="H145" t="s">
         <v>201</v>
       </c>
       <c r="I145" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Dante Suzuki</v>
+        <v>Dante dos Santos</v>
       </c>
       <c r="J145" t="s">
         <v>196</v>
@@ -11187,14 +11187,14 @@
     <row r="146" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G146" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Akemi Matos</v>
+        <v>Camila Severo</v>
       </c>
       <c r="H146" t="s">
         <v>201</v>
       </c>
       <c r="I146" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Fernando Faria</v>
+        <v>Cleber Franca</v>
       </c>
       <c r="J146" t="s">
         <v>196</v>
@@ -11203,14 +11203,14 @@
     <row r="147" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G147" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Irene Lins</v>
+        <v>Jade da Silva</v>
       </c>
       <c r="H147" t="s">
         <v>201</v>
       </c>
       <c r="I147" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Otavio Faria</v>
+        <v>Claudio Takahashi</v>
       </c>
       <c r="J147" t="s">
         <v>196</v>
@@ -11219,14 +11219,14 @@
     <row r="148" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G148" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Sheeva Salgueiro</v>
+        <v>Kitana Alves</v>
       </c>
       <c r="H148" t="s">
         <v>201</v>
       </c>
       <c r="I148" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Bruno Neto</v>
+        <v>Augusto Torres</v>
       </c>
       <c r="J148" t="s">
         <v>196</v>
@@ -11235,14 +11235,14 @@
     <row r="149" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G149" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Rafaela Castanheira</v>
+        <v>Fernanda Alves</v>
       </c>
       <c r="H149" t="s">
         <v>201</v>
       </c>
       <c r="I149" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Morpheu Batista</v>
+        <v>Peterson Suzuki</v>
       </c>
       <c r="J149" t="s">
         <v>196</v>
@@ -11251,14 +11251,14 @@
     <row r="150" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G150" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Sheeva Salgueiro</v>
+        <v>Michele Macedo</v>
       </c>
       <c r="H150" t="s">
         <v>201</v>
       </c>
       <c r="I150" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Cleber Takahashi</v>
+        <v>Peterson Torres</v>
       </c>
       <c r="J150" t="s">
         <v>196</v>
@@ -11267,14 +11267,14 @@
     <row r="151" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G151" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Kitana Macedo</v>
+        <v>Akemi Costa</v>
       </c>
       <c r="H151" t="s">
         <v>201</v>
       </c>
       <c r="I151" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Cauê Batista</v>
+        <v>Morpheu Franca</v>
       </c>
       <c r="J151" t="s">
         <v>196</v>
@@ -11283,14 +11283,14 @@
     <row r="152" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G152" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Trinity Gouveia</v>
+        <v>Jill Pinheiro</v>
       </c>
       <c r="H152" t="s">
         <v>201</v>
       </c>
       <c r="I152" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Jaime Pinheiro</v>
+        <v>Dante Suzuki</v>
       </c>
       <c r="J152" t="s">
         <v>196</v>
@@ -11299,14 +11299,14 @@
     <row r="153" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G153" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Kitana Neves</v>
+        <v>Trinity Takahashi</v>
       </c>
       <c r="H153" t="s">
         <v>201</v>
       </c>
       <c r="I153" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Augusto Semedo</v>
+        <v>Peterson Costa</v>
       </c>
       <c r="J153" t="s">
         <v>196</v>
@@ -11315,14 +11315,14 @@
     <row r="154" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G154" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Jéssica Camilo</v>
+        <v>Odete Takahashi</v>
       </c>
       <c r="H154" t="s">
         <v>201</v>
       </c>
       <c r="I154" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Simão Rocha</v>
+        <v>Eduardo Redfield</v>
       </c>
       <c r="J154" t="s">
         <v>196</v>
@@ -11331,14 +11331,14 @@
     <row r="155" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G155" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Jonas Lins</v>
+        <v>Jéssica Redfield</v>
       </c>
       <c r="H155" t="s">
         <v>201</v>
       </c>
       <c r="I155" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Augusto Pinheiro</v>
+        <v>Cauê Faria</v>
       </c>
       <c r="J155" t="s">
         <v>196</v>
@@ -11347,14 +11347,14 @@
     <row r="156" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G156" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Trinity Hernandes</v>
+        <v>Caroline Tanaka</v>
       </c>
       <c r="H156" t="s">
         <v>201</v>
       </c>
       <c r="I156" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Dante Minazuki</v>
+        <v>Morpheu Alves</v>
       </c>
       <c r="J156" t="s">
         <v>196</v>
@@ -11363,14 +11363,14 @@
     <row r="157" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G157" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Trinity Salgueiro</v>
+        <v>Daniela Matos</v>
       </c>
       <c r="H157" t="s">
         <v>201</v>
       </c>
       <c r="I157" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Otavio Jordão</v>
+        <v>Otavio Faria</v>
       </c>
       <c r="J157" t="s">
         <v>196</v>
@@ -11379,14 +11379,14 @@
     <row r="158" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G158" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Monica Minazuki</v>
+        <v>Rafaela Severo</v>
       </c>
       <c r="H158" t="s">
         <v>201</v>
       </c>
       <c r="I158" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Filipe Gouveia</v>
+        <v>Claudio Hernandes</v>
       </c>
       <c r="J158" t="s">
         <v>196</v>
@@ -11395,14 +11395,14 @@
     <row r="159" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G159" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Sonia Batista</v>
+        <v>Kitana Rocha</v>
       </c>
       <c r="H159" t="s">
         <v>201</v>
       </c>
       <c r="I159" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Claudio Nazário</v>
+        <v>Caio Valverde</v>
       </c>
       <c r="J159" t="s">
         <v>196</v>
@@ -11411,14 +11411,14 @@
     <row r="160" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G160" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Rafaela Neves</v>
+        <v>Jonas Minazuki</v>
       </c>
       <c r="H160" t="s">
         <v>201</v>
       </c>
       <c r="I160" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Leonidas Minazuki</v>
+        <v>Fernando Villablanca</v>
       </c>
       <c r="J160" t="s">
         <v>196</v>
@@ -11427,14 +11427,14 @@
     <row r="161" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G161" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Jill Takahashi</v>
+        <v>Jade Faria</v>
       </c>
       <c r="H161" t="s">
         <v>201</v>
       </c>
       <c r="I161" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Dante Rocha</v>
+        <v>Dante Hernandes</v>
       </c>
       <c r="J161" t="s">
         <v>196</v>
@@ -11443,14 +11443,14 @@
     <row r="162" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G162" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Sarah Faria</v>
+        <v>Tamires Salgueiro</v>
       </c>
       <c r="H162" t="s">
         <v>201</v>
       </c>
       <c r="I162" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Otavio Pinheiro</v>
+        <v>Eric Leal</v>
       </c>
       <c r="J162" t="s">
         <v>196</v>
@@ -11459,14 +11459,14 @@
     <row r="163" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G163" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Fernanda Lins</v>
+        <v>Lara Pinheiro</v>
       </c>
       <c r="H163" t="s">
         <v>201</v>
       </c>
       <c r="I163" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eric Neto</v>
+        <v>Cleber dos Santos</v>
       </c>
       <c r="J163" t="s">
         <v>196</v>
@@ -11475,14 +11475,14 @@
     <row r="164" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G164" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Rafaela Semedo</v>
+        <v>Irene Ishida</v>
       </c>
       <c r="H164" t="s">
         <v>201</v>
       </c>
       <c r="I164" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Jaime Alves</v>
+        <v>Yori Valverde</v>
       </c>
       <c r="J164" t="s">
         <v>196</v>
@@ -11491,14 +11491,14 @@
     <row r="165" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G165" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Yoko Yamada</v>
+        <v>Barbara Takahashi</v>
       </c>
       <c r="H165" t="s">
         <v>201</v>
       </c>
       <c r="I165" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Jaime Salgueiro</v>
+        <v>Bruno da Silva</v>
       </c>
       <c r="J165" t="s">
         <v>196</v>
@@ -11507,14 +11507,14 @@
     <row r="166" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G166" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Michele Camilo</v>
+        <v>Lara Takahashi</v>
       </c>
       <c r="H166" t="s">
         <v>201</v>
       </c>
       <c r="I166" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Cleber Peixoto</v>
+        <v>Peterson Pinheiro</v>
       </c>
       <c r="J166" t="s">
         <v>196</v>
@@ -11523,14 +11523,14 @@
     <row r="167" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G167" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Camila da Silva</v>
+        <v>Kitana Monteiro</v>
       </c>
       <c r="H167" t="s">
         <v>201</v>
       </c>
       <c r="I167" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Augusto Neves</v>
+        <v>Augusto Redfield</v>
       </c>
       <c r="J167" t="s">
         <v>196</v>
@@ -11539,14 +11539,14 @@
     <row r="168" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G168" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Monica Jordão</v>
+        <v>Aline Nazário</v>
       </c>
       <c r="H168" t="s">
         <v>201</v>
       </c>
       <c r="I168" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eric Pinheiro</v>
+        <v>Cleber Takahashi</v>
       </c>
       <c r="J168" t="s">
         <v>196</v>
@@ -11555,14 +11555,14 @@
     <row r="169" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G169" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Odete Severo</v>
+        <v>Barbara Neves</v>
       </c>
       <c r="H169" t="s">
         <v>201</v>
       </c>
       <c r="I169" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Peterson Villablanca</v>
+        <v>Yori Torres</v>
       </c>
       <c r="J169" t="s">
         <v>196</v>
@@ -11571,14 +11571,14 @@
     <row r="170" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G170" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Bruna Minazuki</v>
+        <v>Jade Macedo</v>
       </c>
       <c r="H170" t="s">
         <v>201</v>
       </c>
       <c r="I170" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Caio Villablanca</v>
+        <v>Doulgas Franca</v>
       </c>
       <c r="J170" t="s">
         <v>196</v>
@@ -11587,14 +11587,14 @@
     <row r="171" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G171" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Sarah Minazuki</v>
+        <v>Sheeva Tanaka</v>
       </c>
       <c r="H171" t="s">
         <v>201</v>
       </c>
       <c r="I171" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Jaime Torres</v>
+        <v>Bruno da Silva</v>
       </c>
       <c r="J171" t="s">
         <v>196</v>
@@ -11603,14 +11603,14 @@
     <row r="172" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G172" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Camila Jordão</v>
+        <v>Milena Salgueiro</v>
       </c>
       <c r="H172" t="s">
         <v>201</v>
       </c>
       <c r="I172" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Claudio Torres</v>
+        <v>Eric Leal</v>
       </c>
       <c r="J172" t="s">
         <v>196</v>
@@ -11619,14 +11619,14 @@
     <row r="173" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G173" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Michele Redfield</v>
+        <v>Milena Neto</v>
       </c>
       <c r="H173" t="s">
         <v>201</v>
       </c>
       <c r="I173" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Otavio Castanheira</v>
+        <v>Eduardo Jordão</v>
       </c>
       <c r="J173" t="s">
         <v>196</v>
@@ -11635,14 +11635,14 @@
     <row r="174" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G174" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Daniela Gouveia</v>
+        <v>Yoko Pádua</v>
       </c>
       <c r="H174" t="s">
         <v>201</v>
       </c>
       <c r="I174" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Peterson Neto</v>
+        <v>Cauê Pinheiro</v>
       </c>
       <c r="J174" t="s">
         <v>196</v>
@@ -11651,14 +11651,14 @@
     <row r="175" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G175" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Odete Semedo</v>
+        <v>Trinity Franca</v>
       </c>
       <c r="H175" t="s">
         <v>201</v>
       </c>
       <c r="I175" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eric Monteiro</v>
+        <v>Fernando Neves</v>
       </c>
       <c r="J175" t="s">
         <v>196</v>
@@ -11667,14 +11667,14 @@
     <row r="176" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G176" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Jill Lins</v>
+        <v>Tamires Neves</v>
       </c>
       <c r="H176" t="s">
         <v>201</v>
       </c>
       <c r="I176" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Jaime Sato</v>
+        <v>Filipe Tanaka</v>
       </c>
       <c r="J176" t="s">
         <v>196</v>
@@ -11683,14 +11683,14 @@
     <row r="177" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G177" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Milena Rocha</v>
+        <v>Tamires Faria</v>
       </c>
       <c r="H177" t="s">
         <v>201</v>
       </c>
       <c r="I177" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Bruno Franca</v>
+        <v>Dante Lins</v>
       </c>
       <c r="J177" t="s">
         <v>196</v>
@@ -11699,14 +11699,14 @@
     <row r="178" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G178" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Sonia Peixoto</v>
+        <v>Kitana Takahashi</v>
       </c>
       <c r="H178" t="s">
         <v>201</v>
       </c>
       <c r="I178" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Filipe Redfield</v>
+        <v>Claudio Valverde</v>
       </c>
       <c r="J178" t="s">
         <v>196</v>
@@ -11715,14 +11715,14 @@
     <row r="179" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G179" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Fernanda da Silva</v>
+        <v>Camila Pádua</v>
       </c>
       <c r="H179" t="s">
         <v>201</v>
       </c>
       <c r="I179" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Xerxes Faria</v>
+        <v>Cleber Carvalho</v>
       </c>
       <c r="J179" t="s">
         <v>196</v>
@@ -11731,14 +11731,14 @@
     <row r="180" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G180" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ChunLi Redfield</v>
+        <v>Milena Torres</v>
       </c>
       <c r="H180" t="s">
         <v>201</v>
       </c>
       <c r="I180" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Xerxes Semedo</v>
+        <v>Claudio Matos</v>
       </c>
       <c r="J180" t="s">
         <v>196</v>
@@ -11747,14 +11747,14 @@
     <row r="181" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G181" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Angelina dos Santos</v>
+        <v>Aline Alves</v>
       </c>
       <c r="H181" t="s">
         <v>201</v>
       </c>
       <c r="I181" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eric Takahashi</v>
+        <v>Jaime Takahashi</v>
       </c>
       <c r="J181" t="s">
         <v>196</v>
@@ -11763,14 +11763,14 @@
     <row r="182" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G182" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Trinity Neto</v>
+        <v>Daniela Leal</v>
       </c>
       <c r="H182" t="s">
         <v>201</v>
       </c>
       <c r="I182" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eduardo Redfield</v>
+        <v>Cauê Lins</v>
       </c>
       <c r="J182" t="s">
         <v>196</v>
@@ -11779,14 +11779,14 @@
     <row r="183" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G183" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Kitana Alves</v>
+        <v>Yoko da Silva</v>
       </c>
       <c r="H183" t="s">
         <v>201</v>
       </c>
       <c r="I183" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eduardo Rocha</v>
+        <v>Claudio dos Santos</v>
       </c>
       <c r="J183" t="s">
         <v>196</v>
@@ -11795,14 +11795,14 @@
     <row r="184" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G184" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Camila Torres</v>
+        <v>Sarah Lins</v>
       </c>
       <c r="H184" t="s">
         <v>201</v>
       </c>
       <c r="I184" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Claudio Hernandes</v>
+        <v>Filipe Carvalho</v>
       </c>
       <c r="J184" t="s">
         <v>196</v>
@@ -11811,14 +11811,14 @@
     <row r="185" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G185" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Kitana Neto</v>
+        <v>Angelina Villablanca</v>
       </c>
       <c r="H185" t="s">
         <v>201</v>
       </c>
       <c r="I185" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Xerxes Minazuki</v>
+        <v>Bruno Lins</v>
       </c>
       <c r="J185" t="s">
         <v>196</v>
@@ -11827,14 +11827,14 @@
     <row r="186" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G186" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Sonia Batista</v>
+        <v>Barbara Salgueiro</v>
       </c>
       <c r="H186" t="s">
         <v>201</v>
       </c>
       <c r="I186" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Jaime Castanheira</v>
+        <v>Eric Neves</v>
       </c>
       <c r="J186" t="s">
         <v>196</v>
@@ -11843,14 +11843,14 @@
     <row r="187" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G187" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Akemi Redfield</v>
+        <v>Andreia Leal</v>
       </c>
       <c r="H187" t="s">
         <v>201</v>
       </c>
       <c r="I187" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Simão Neves</v>
+        <v>Claudio Franca</v>
       </c>
       <c r="J187" t="s">
         <v>196</v>
@@ -11859,14 +11859,14 @@
     <row r="188" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G188" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Fernanda Matos</v>
+        <v>Fernanda Neto</v>
       </c>
       <c r="H188" t="s">
         <v>201</v>
       </c>
       <c r="I188" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Doulgas Torres</v>
+        <v>Simão Suzuki</v>
       </c>
       <c r="J188" t="s">
         <v>196</v>
@@ -11875,14 +11875,14 @@
     <row r="189" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G189" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Rafaela Macedo</v>
+        <v>Lara Pádua</v>
       </c>
       <c r="H189" t="s">
         <v>201</v>
       </c>
       <c r="I189" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eric Hernandes</v>
+        <v>Filipe Franca</v>
       </c>
       <c r="J189" t="s">
         <v>196</v>
@@ -11891,14 +11891,14 @@
     <row r="190" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G190" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Michele Valentine</v>
+        <v>Angelina Neto</v>
       </c>
       <c r="H190" t="s">
         <v>201</v>
       </c>
       <c r="I190" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Cauê Monteiro</v>
+        <v>Eduardo Salgueiro</v>
       </c>
       <c r="J190" t="s">
         <v>196</v>
@@ -11907,14 +11907,14 @@
     <row r="191" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G191" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Odete Torres</v>
+        <v>Rafaela Sato</v>
       </c>
       <c r="H191" t="s">
         <v>201</v>
       </c>
       <c r="I191" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Xerxes Peixoto</v>
+        <v>Jaime Alves</v>
       </c>
       <c r="J191" t="s">
         <v>196</v>
@@ -11923,14 +11923,14 @@
     <row r="192" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G192" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Kitana Ishida</v>
+        <v>Jéssica da Silva</v>
       </c>
       <c r="H192" t="s">
         <v>201</v>
       </c>
       <c r="I192" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Jaime Neves</v>
+        <v>Leonidas Neto</v>
       </c>
       <c r="J192" t="s">
         <v>196</v>
@@ -11939,14 +11939,14 @@
     <row r="193" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G193" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Andreia Gouveia</v>
+        <v>Jéssica Pinheiro</v>
       </c>
       <c r="H193" t="s">
         <v>201</v>
       </c>
       <c r="I193" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Xerxes Leal</v>
+        <v>Peterson Costa</v>
       </c>
       <c r="J193" t="s">
         <v>196</v>
@@ -11955,14 +11955,14 @@
     <row r="194" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G194" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Akemi Faria</v>
+        <v>Trinity Takahashi</v>
       </c>
       <c r="H194" t="s">
         <v>201</v>
       </c>
       <c r="I194" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Claudio Jordão</v>
+        <v>Bruno Alves</v>
       </c>
       <c r="J194" t="s">
         <v>196</v>
@@ -11971,14 +11971,14 @@
     <row r="195" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G195" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Rafaela Peixoto</v>
+        <v>Rafaela da Silva</v>
       </c>
       <c r="H195" t="s">
         <v>201</v>
       </c>
       <c r="I195" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Eduardo Gouveia</v>
+        <v>Eric Jordão</v>
       </c>
       <c r="J195" t="s">
         <v>196</v>
@@ -11987,14 +11987,14 @@
     <row r="196" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G196" t="str">
         <f t="shared" ref="G196:G201" ca="1" si="6">CONCATENATE(VLOOKUP(RANDBETWEEN(1,30),$A$1:$B$31,2,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Sarah Salgueiro</v>
+        <v>ChunLi Faria</v>
       </c>
       <c r="H196" t="s">
         <v>201</v>
       </c>
       <c r="I196" t="str">
         <f t="shared" ref="I196:I201" ca="1" si="7">CONCATENATE(VLOOKUP(RANDBETWEEN(1,20),$A$1:$C$21,3,FALSE)," ",VLOOKUP(RANDBETWEEN(1,45),$A$1:$D$46,4,FALSE))</f>
-        <v>Xerxes Semedo</v>
+        <v>Dante Pinheiro</v>
       </c>
       <c r="J196" t="s">
         <v>196</v>
@@ -12003,14 +12003,14 @@
     <row r="197" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G197" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>Michele da Silva</v>
+        <v>Michele Neto</v>
       </c>
       <c r="H197" t="s">
         <v>201</v>
       </c>
       <c r="I197" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Yori Jordão</v>
+        <v>Doulgas Tanaka</v>
       </c>
       <c r="J197" t="s">
         <v>196</v>
@@ -12019,14 +12019,14 @@
     <row r="198" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G198" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>Michele Takahashi</v>
+        <v>Caroline Valentine</v>
       </c>
       <c r="H198" t="s">
         <v>201</v>
       </c>
       <c r="I198" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Otavio da Silva</v>
+        <v>Dante Faria</v>
       </c>
       <c r="J198" t="s">
         <v>196</v>
@@ -12035,14 +12035,14 @@
     <row r="199" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G199" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>Bruna Alves</v>
+        <v>Aline Suzuki</v>
       </c>
       <c r="H199" t="s">
         <v>201</v>
       </c>
       <c r="I199" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Peterson Faria</v>
+        <v>Claudio Neto</v>
       </c>
       <c r="J199" t="s">
         <v>196</v>
@@ -12051,14 +12051,14 @@
     <row r="200" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G200" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>Yoko Pinheiro</v>
+        <v>Rafaela Alves</v>
       </c>
       <c r="H200" t="s">
         <v>201</v>
       </c>
       <c r="I200" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Peterson Costa</v>
+        <v>Bruno Hernandes</v>
       </c>
       <c r="J200" t="s">
         <v>196</v>
@@ -12067,14 +12067,14 @@
     <row r="201" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G201" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>Bruna dos Santos</v>
+        <v>Caroline Franca</v>
       </c>
       <c r="H201" t="s">
         <v>201</v>
       </c>
       <c r="I201" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Cleber da Silva</v>
+        <v>Leonidas Valverde</v>
       </c>
       <c r="J201" t="s">
         <v>196</v>
@@ -12563,7 +12563,7 @@
       <c r="P2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3" t="str">
-        <f t="shared" ref="Q2:Y17" si="0">SUBSTITUTE(R2,H$1,H2,1)</f>
+        <f t="shared" ref="S2:Y17" si="0">SUBSTITUTE(R2,H$1,H2,1)</f>
         <v/>
       </c>
       <c r="T2" s="3" t="str">
@@ -20842,7 +20842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI253"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AD17" sqref="AD17"/>
     </sheetView>

</xml_diff>